<commit_message>
Økonomisk analyse opdateret med Excel
</commit_message>
<xml_diff>
--- a/Rapportskrivning/Bilag/Til Projektrapport/Økonomi/Økonomi - tal.xlsx
+++ b/Rapportskrivning/Bilag/Til Projektrapport/Økonomi/Økonomi - tal.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Charlotte\Documents\Bachelor\Rapportskrivning\Bilag\Til Projektrapport\Økonomi\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Charlotte\Documents\Automatic-Sonography\Rapportskrivning\Bilag\Til Projektrapport\Økonomi\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="55">
   <si>
     <t>Engangsudgifter til afskrivning</t>
   </si>
@@ -86,9 +86,6 @@
     <t xml:space="preserve">Tidforbrug </t>
   </si>
   <si>
-    <t>Ultralydsscreening</t>
-  </si>
-  <si>
     <t>min</t>
   </si>
   <si>
@@ -98,9 +95,6 @@
     <t>3D billede og konvertering</t>
   </si>
   <si>
-    <t>Udgifter screening (UR10 Robot)</t>
-  </si>
-  <si>
     <t>Check af billeder (radiolog)</t>
   </si>
   <si>
@@ -113,21 +107,12 @@
     <t>Transport</t>
   </si>
   <si>
-    <t xml:space="preserve">Hvor mange screeninger før betalt af? </t>
-  </si>
-  <si>
-    <t>Udgifter screening (Anvendt)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Fund: hvis transporttid er under 4 minutter vil det aldrig give positiv BC. </t>
   </si>
   <si>
     <t xml:space="preserve">Overslag af priser </t>
   </si>
   <si>
-    <t xml:space="preserve">Antal screeninger </t>
-  </si>
-  <si>
     <t>Transport (min)</t>
   </si>
   <si>
@@ -167,9 +152,6 @@
     <t>Serviceaftale (årlig)</t>
   </si>
   <si>
-    <t>Breakeven (Screeninger)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Afskrivning </t>
   </si>
   <si>
@@ -182,25 +164,31 @@
     <t xml:space="preserve">FO (i alt) </t>
   </si>
   <si>
-    <t>Årlig pris</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hvor meget koster UR10 robotten årligt? </t>
-  </si>
-  <si>
-    <t xml:space="preserve">(Afskrivning af robot) </t>
-  </si>
-  <si>
-    <t>år</t>
-  </si>
-  <si>
-    <t>Ultralydsscreeninger</t>
-  </si>
-  <si>
-    <t>Pris for én ultralydsscreening</t>
-  </si>
-  <si>
     <t>Computer</t>
+  </si>
+  <si>
+    <t>Antal scanninger</t>
+  </si>
+  <si>
+    <t>Pris for én ultralydsscaninger</t>
+  </si>
+  <si>
+    <t>Ultralydsscanning</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Antal scanninger </t>
+  </si>
+  <si>
+    <t>Breakeven (Scanninger)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hvor mange scanninger før betalt af? </t>
+  </si>
+  <si>
+    <t>Udgifter scanning (UR10 Robot)</t>
+  </si>
+  <si>
+    <t>Udgifter scanning (Anvendt)</t>
   </si>
 </sst>
 </file>
@@ -288,7 +276,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -312,7 +300,6 @@
     <xf numFmtId="43" fontId="0" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -320,6 +307,14 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -639,7 +634,7 @@
   <dimension ref="A1:U46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="G1" sqref="G1:K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -660,32 +655,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="G1" s="23" t="s">
-        <v>33</v>
-      </c>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-      <c r="K1" s="23"/>
-      <c r="L1" s="23"/>
-      <c r="M1" s="23" t="s">
-        <v>52</v>
-      </c>
-      <c r="N1" s="23"/>
-      <c r="O1" s="23"/>
-      <c r="P1" s="23"/>
-      <c r="Q1" s="23"/>
-      <c r="R1" s="23"/>
-      <c r="S1" s="23"/>
-      <c r="T1" s="23"/>
-      <c r="U1" s="23"/>
+      <c r="A1" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="G1" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="25"/>
+      <c r="N1" s="25"/>
+      <c r="O1" s="25"/>
+      <c r="P1" s="25"/>
+      <c r="Q1" s="25"/>
+      <c r="R1" s="25"/>
+      <c r="S1" s="25"/>
+      <c r="T1" s="25"/>
+      <c r="U1" s="25"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
@@ -701,11 +694,17 @@
         <v>10</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="M2" s="19" t="s">
-        <v>53</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="M2" s="24"/>
+      <c r="N2" s="11"/>
+      <c r="O2" s="11"/>
+      <c r="P2" s="11"/>
+      <c r="Q2" s="11"/>
+      <c r="R2" s="11"/>
+      <c r="S2" s="11"/>
+      <c r="T2" s="11"/>
+      <c r="U2" s="11"/>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -721,22 +720,22 @@
         <v>369</v>
       </c>
       <c r="G3" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="H3" s="3">
         <f>B35</f>
         <v>201668</v>
       </c>
       <c r="I3" s="3"/>
-      <c r="M3" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="P3">
-        <v>10</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>55</v>
-      </c>
+      <c r="M3" s="11"/>
+      <c r="N3" s="11"/>
+      <c r="O3" s="11"/>
+      <c r="P3" s="11"/>
+      <c r="Q3" s="11"/>
+      <c r="R3" s="11"/>
+      <c r="S3" s="11"/>
+      <c r="T3" s="11"/>
+      <c r="U3" s="11"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -752,19 +751,22 @@
         <v>173</v>
       </c>
       <c r="G4" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="H4" s="3">
         <f>B41</f>
         <v>10759</v>
       </c>
       <c r="J4" s="3"/>
-      <c r="M4" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="P4">
-        <v>2300</v>
-      </c>
+      <c r="M4" s="11"/>
+      <c r="N4" s="11"/>
+      <c r="O4" s="11"/>
+      <c r="P4" s="11"/>
+      <c r="Q4" s="11"/>
+      <c r="R4" s="11"/>
+      <c r="S4" s="11"/>
+      <c r="T4" s="11"/>
+      <c r="U4" s="11"/>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -780,34 +782,52 @@
         <v>700</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="H5" s="4">
         <f>B46</f>
         <v>6768</v>
       </c>
+      <c r="M5" s="11"/>
+      <c r="N5" s="11"/>
+      <c r="O5" s="11"/>
+      <c r="P5" s="11"/>
+      <c r="Q5" s="11"/>
+      <c r="R5" s="11"/>
+      <c r="S5" s="11"/>
+      <c r="T5" s="11"/>
+      <c r="U5" s="11"/>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="B6" s="1">
         <v>4999</v>
       </c>
       <c r="D6" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="E6" s="1">
         <v>1000</v>
       </c>
       <c r="G6" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="H6" s="3">
         <f>SUM(H3:H5)</f>
         <v>219195</v>
       </c>
       <c r="J6" s="10"/>
+      <c r="M6" s="11"/>
+      <c r="N6" s="11"/>
+      <c r="O6" s="11"/>
+      <c r="P6" s="11"/>
+      <c r="Q6" s="11"/>
+      <c r="R6" s="11"/>
+      <c r="S6" s="11"/>
+      <c r="T6" s="11"/>
+      <c r="U6" s="11"/>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -817,11 +837,20 @@
         <v>700</v>
       </c>
       <c r="D7" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E7">
         <v>2</v>
       </c>
+      <c r="M7" s="11"/>
+      <c r="N7" s="11"/>
+      <c r="O7" s="11"/>
+      <c r="P7" s="11"/>
+      <c r="Q7" s="11"/>
+      <c r="R7" s="11"/>
+      <c r="S7" s="11"/>
+      <c r="T7" s="11"/>
+      <c r="U7" s="11"/>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -831,66 +860,111 @@
         <v>500</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="E8">
         <f>300*1/1000*E7</f>
         <v>0.6</v>
       </c>
       <c r="G8" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="H8" s="1">
         <f>H6/(E27-B27)</f>
         <v>636.26380005998976</v>
       </c>
+      <c r="M8" s="11"/>
+      <c r="N8" s="11"/>
+      <c r="O8" s="11"/>
+      <c r="P8" s="11"/>
+      <c r="Q8" s="11"/>
+      <c r="R8" s="11"/>
+      <c r="S8" s="11"/>
+      <c r="T8" s="11"/>
+      <c r="U8" s="11"/>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B9" s="1">
         <v>7500</v>
       </c>
       <c r="D9" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="E9">
         <f>300*1/1000*E7</f>
         <v>0.6</v>
       </c>
+      <c r="M9" s="11"/>
+      <c r="N9" s="11"/>
+      <c r="O9" s="11"/>
+      <c r="P9" s="11"/>
+      <c r="Q9" s="11"/>
+      <c r="R9" s="11"/>
+      <c r="S9" s="11"/>
+      <c r="T9" s="11"/>
+      <c r="U9" s="11"/>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="I10" s="3">
         <f>SUM(I6:I9)</f>
         <v>0</v>
       </c>
+      <c r="M10" s="11"/>
+      <c r="N10" s="11"/>
+      <c r="O10" s="11"/>
+      <c r="P10" s="11"/>
+      <c r="Q10" s="11"/>
+      <c r="R10" s="11"/>
+      <c r="S10" s="11"/>
+      <c r="T10" s="11"/>
+      <c r="U10" s="11"/>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B11" s="1"/>
+      <c r="M11" s="11"/>
+      <c r="N11" s="11"/>
+      <c r="O11" s="11"/>
+      <c r="P11" s="11"/>
+      <c r="Q11" s="11"/>
+      <c r="R11" s="11"/>
+      <c r="S11" s="11"/>
+      <c r="T11" s="11"/>
+      <c r="U11" s="11"/>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12" s="20" t="s">
         <v>21</v>
+      </c>
+      <c r="B12" s="19" t="s">
+        <v>20</v>
       </c>
       <c r="C12" s="12"/>
       <c r="D12" s="5" t="s">
         <v>19</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G12" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="H12" s="7"/>
+      <c r="M12" s="11"/>
+      <c r="N12" s="11"/>
+      <c r="O12" s="11"/>
+      <c r="P12" s="11"/>
+      <c r="Q12" s="11"/>
+      <c r="R12" s="11"/>
+      <c r="S12" s="11"/>
+      <c r="T12" s="11"/>
+      <c r="U12" s="11"/>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B13" s="1">
         <v>10</v>
@@ -903,24 +977,33 @@
         <v>10</v>
       </c>
       <c r="G13" s="11" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="H13" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="I13" s="11" t="s">
-        <v>33</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="M13" s="11"/>
+      <c r="N13" s="11"/>
+      <c r="O13" s="11"/>
+      <c r="P13" s="11"/>
+      <c r="Q13" s="11"/>
+      <c r="R13" s="11"/>
+      <c r="S13" s="11"/>
+      <c r="T13" s="11"/>
+      <c r="U13" s="11"/>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B14" s="1">
         <v>2</v>
       </c>
       <c r="D14" t="s">
-        <v>20</v>
+        <v>49</v>
       </c>
       <c r="E14">
         <v>4</v>
@@ -934,16 +1017,25 @@
       <c r="I14" s="1">
         <v>2121241.94</v>
       </c>
+      <c r="M14" s="11"/>
+      <c r="N14" s="11"/>
+      <c r="O14" s="11"/>
+      <c r="P14" s="11"/>
+      <c r="Q14" s="11"/>
+      <c r="R14" s="11"/>
+      <c r="S14" s="11"/>
+      <c r="T14" s="11"/>
+      <c r="U14" s="11"/>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>20</v>
+        <v>49</v>
       </c>
       <c r="B15" s="1">
         <v>5</v>
       </c>
       <c r="D15" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E15">
         <v>60</v>
@@ -957,10 +1049,19 @@
       <c r="I15" s="1">
         <v>35052.51</v>
       </c>
+      <c r="M15" s="11"/>
+      <c r="N15" s="11"/>
+      <c r="O15" s="11"/>
+      <c r="P15" s="11"/>
+      <c r="Q15" s="11"/>
+      <c r="R15" s="11"/>
+      <c r="S15" s="11"/>
+      <c r="T15" s="11"/>
+      <c r="U15" s="11"/>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B16" s="1">
         <v>10</v>
@@ -974,10 +1075,19 @@
       <c r="I16" s="1">
         <v>8873.09</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="M16" s="11"/>
+      <c r="N16" s="11"/>
+      <c r="O16" s="11"/>
+      <c r="P16" s="11"/>
+      <c r="Q16" s="11"/>
+      <c r="R16" s="11"/>
+      <c r="S16" s="11"/>
+      <c r="T16" s="11"/>
+      <c r="U16" s="11"/>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B17" s="1">
         <f>4*60</f>
@@ -992,8 +1102,17 @@
       <c r="I17" s="1">
         <v>5923.66</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="M17" s="11"/>
+      <c r="N17" s="11"/>
+      <c r="O17" s="11"/>
+      <c r="P17" s="11"/>
+      <c r="Q17" s="11"/>
+      <c r="R17" s="11"/>
+      <c r="S17" s="11"/>
+      <c r="T17" s="11"/>
+      <c r="U17" s="11"/>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="G18" s="11">
         <v>15</v>
       </c>
@@ -1003,17 +1122,26 @@
       <c r="I18" s="1">
         <v>3235.19</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="M18" s="11"/>
+      <c r="N18" s="11"/>
+      <c r="O18" s="11"/>
+      <c r="P18" s="11"/>
+      <c r="Q18" s="11"/>
+      <c r="R18" s="11"/>
+      <c r="S18" s="11"/>
+      <c r="T18" s="11"/>
+      <c r="U18" s="11"/>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B19" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="B19" s="19" t="s">
         <v>10</v>
       </c>
       <c r="C19" s="12"/>
       <c r="D19" s="5" t="s">
-        <v>30</v>
+        <v>54</v>
       </c>
       <c r="E19" s="5" t="s">
         <v>10</v>
@@ -1027,8 +1155,17 @@
       <c r="I19" s="1">
         <v>2225.25</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="M19" s="11"/>
+      <c r="N19" s="11"/>
+      <c r="O19" s="11"/>
+      <c r="P19" s="11"/>
+      <c r="Q19" s="11"/>
+      <c r="R19" s="11"/>
+      <c r="S19" s="11"/>
+      <c r="T19" s="11"/>
+      <c r="U19" s="11"/>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" t="str">
         <f>A13</f>
         <v xml:space="preserve">Forberedelse (snak mm) </v>
@@ -1054,10 +1191,19 @@
       <c r="I20" s="1">
         <v>1369.94</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="M20" s="11"/>
+      <c r="N20" s="11"/>
+      <c r="O20" s="11"/>
+      <c r="P20" s="11"/>
+      <c r="Q20" s="11"/>
+      <c r="R20" s="11"/>
+      <c r="S20" s="11"/>
+      <c r="T20" s="11"/>
+      <c r="U20" s="11"/>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B21" s="1">
         <f>B14*E4/60</f>
@@ -1065,7 +1211,7 @@
       </c>
       <c r="D21" t="str">
         <f>D14</f>
-        <v>Ultralydsscreening</v>
+        <v>Ultralydsscanning</v>
       </c>
       <c r="E21">
         <f>E14*E3/60</f>
@@ -1080,18 +1226,27 @@
       <c r="I21" s="1">
         <v>868.95</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="M21" s="11"/>
+      <c r="N21" s="11"/>
+      <c r="O21" s="11"/>
+      <c r="P21" s="11"/>
+      <c r="Q21" s="11"/>
+      <c r="R21" s="11"/>
+      <c r="S21" s="11"/>
+      <c r="T21" s="11"/>
+      <c r="U21" s="11"/>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22" t="str">
         <f>A15</f>
-        <v>Ultralydsscreening</v>
+        <v>Ultralydsscanning</v>
       </c>
       <c r="B22" s="1">
         <f>B15*E4/60</f>
         <v>14.416666666666666</v>
       </c>
       <c r="D22" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="E22">
         <f>E9*E14/60</f>
@@ -1106,8 +1261,17 @@
       <c r="I22" s="1">
         <v>636.26</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="M22" s="11"/>
+      <c r="N22" s="11"/>
+      <c r="O22" s="11"/>
+      <c r="P22" s="11"/>
+      <c r="Q22" s="11"/>
+      <c r="R22" s="11"/>
+      <c r="S22" s="11"/>
+      <c r="T22" s="11"/>
+      <c r="U22" s="11"/>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23" t="str">
         <f>A16</f>
         <v>Check af billeder (radiolog)</v>
@@ -1124,62 +1288,126 @@
         <f>E15/60*E3</f>
         <v>369</v>
       </c>
+      <c r="G23" s="23"/>
       <c r="H23" s="1"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="M23" s="11"/>
+      <c r="N23" s="11"/>
+      <c r="O23" s="11"/>
+      <c r="P23" s="11"/>
+      <c r="Q23" s="11"/>
+      <c r="R23" s="11"/>
+      <c r="S23" s="11"/>
+      <c r="T23" s="11"/>
+      <c r="U23" s="11"/>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B24" s="1">
         <f>E8*(B15+B14)/60</f>
         <v>7.0000000000000007E-2</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="M24" s="11"/>
+      <c r="N24" s="11"/>
+      <c r="O24" s="11"/>
+      <c r="P24" s="11"/>
+      <c r="Q24" s="11"/>
+      <c r="R24" s="11"/>
+      <c r="S24" s="11"/>
+      <c r="T24" s="11"/>
+      <c r="U24" s="11"/>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B25" s="1">
         <f>B15*E9/60</f>
         <v>0.05</v>
       </c>
       <c r="H25" s="1"/>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="M25" s="11"/>
+      <c r="N25" s="11"/>
+      <c r="O25" s="11"/>
+      <c r="P25" s="11"/>
+      <c r="Q25" s="11"/>
+      <c r="R25" s="11"/>
+      <c r="S25" s="11"/>
+      <c r="T25" s="11"/>
+      <c r="U25" s="11"/>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="8"/>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
       <c r="H26" s="1"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="M26" s="11"/>
+      <c r="N26" s="11"/>
+      <c r="O26" s="11"/>
+      <c r="P26" s="11"/>
+      <c r="Q26" s="11"/>
+      <c r="R26" s="11"/>
+      <c r="S26" s="11"/>
+      <c r="T26" s="11"/>
+      <c r="U26" s="11"/>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B27" s="1">
         <f>SUM(B20:B25)</f>
         <v>110.63666666666666</v>
       </c>
       <c r="D27" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E27">
         <f>SUM(E20:E25)</f>
         <v>455.14</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="M27" s="11"/>
+      <c r="N27" s="11"/>
+      <c r="O27" s="11"/>
+      <c r="P27" s="11"/>
+      <c r="Q27" s="11"/>
+      <c r="R27" s="11"/>
+      <c r="S27" s="11"/>
+      <c r="T27" s="11"/>
+      <c r="U27" s="11"/>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B28" s="1"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="M28" s="11"/>
+      <c r="N28" s="11"/>
+      <c r="O28" s="11"/>
+      <c r="P28" s="11"/>
+      <c r="Q28" s="11"/>
+      <c r="R28" s="11"/>
+      <c r="S28" s="11"/>
+      <c r="T28" s="11"/>
+      <c r="U28" s="11"/>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B29" s="20" t="s">
+      <c r="B29" s="19" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="M29" s="11"/>
+      <c r="N29" s="11"/>
+      <c r="O29" s="11"/>
+      <c r="P29" s="11"/>
+      <c r="Q29" s="11"/>
+      <c r="R29" s="11"/>
+      <c r="S29" s="11"/>
+      <c r="T29" s="11"/>
+      <c r="U29" s="11"/>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>1</v>
       </c>
@@ -1187,8 +1415,17 @@
         <f>B3</f>
         <v>195000</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="M30" s="11"/>
+      <c r="N30" s="11"/>
+      <c r="O30" s="11"/>
+      <c r="P30" s="11"/>
+      <c r="Q30" s="11"/>
+      <c r="R30" s="11"/>
+      <c r="S30" s="11"/>
+      <c r="T30" s="11"/>
+      <c r="U30" s="11"/>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>2</v>
       </c>
@@ -1196,8 +1433,17 @@
         <f>B4</f>
         <v>849</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="M31" s="11"/>
+      <c r="N31" s="11"/>
+      <c r="O31" s="11"/>
+      <c r="P31" s="11"/>
+      <c r="Q31" s="11"/>
+      <c r="R31" s="11"/>
+      <c r="S31" s="11"/>
+      <c r="T31" s="11"/>
+      <c r="U31" s="11"/>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>3</v>
       </c>
@@ -1205,8 +1451,17 @@
         <f>B5</f>
         <v>120</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="M32" s="11"/>
+      <c r="N32" s="11"/>
+      <c r="O32" s="11"/>
+      <c r="P32" s="11"/>
+      <c r="Q32" s="11"/>
+      <c r="R32" s="11"/>
+      <c r="S32" s="11"/>
+      <c r="T32" s="11"/>
+      <c r="U32" s="11"/>
+    </row>
+    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>13</v>
       </c>
@@ -1214,8 +1469,17 @@
         <f>B6</f>
         <v>4999</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="M33" s="11"/>
+      <c r="N33" s="11"/>
+      <c r="O33" s="11"/>
+      <c r="P33" s="11"/>
+      <c r="Q33" s="11"/>
+      <c r="R33" s="11"/>
+      <c r="S33" s="11"/>
+      <c r="T33" s="11"/>
+      <c r="U33" s="11"/>
+    </row>
+    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>15</v>
       </c>
@@ -1223,22 +1487,51 @@
         <f>B7</f>
         <v>700</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="M34" s="11"/>
+      <c r="N34" s="11"/>
+      <c r="O34" s="11"/>
+      <c r="P34" s="11"/>
+      <c r="Q34" s="11"/>
+      <c r="R34" s="11"/>
+      <c r="S34" s="11"/>
+      <c r="T34" s="11"/>
+      <c r="U34" s="11"/>
+    </row>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B35" s="1">
         <f>SUM(B30:B34)</f>
         <v>201668</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="M35" s="11"/>
+      <c r="N35" s="11"/>
+      <c r="O35" s="11"/>
+      <c r="P35" s="11"/>
+      <c r="Q35" s="11"/>
+      <c r="R35" s="11"/>
+      <c r="S35" s="11"/>
+      <c r="T35" s="11"/>
+      <c r="U35" s="11"/>
+    </row>
+    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="M36" s="11"/>
+      <c r="N36" s="11"/>
+      <c r="O36" s="11"/>
+      <c r="P36" s="11"/>
+      <c r="Q36" s="11"/>
+      <c r="R36" s="11"/>
+      <c r="S36" s="11"/>
+      <c r="T36" s="11"/>
+      <c r="U36" s="11"/>
+    </row>
+    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B37" s="20" t="s">
+      <c r="B37" s="19" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>5</v>
       </c>
@@ -1246,7 +1539,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A39" s="13" t="s">
         <v>12</v>
       </c>
@@ -1255,51 +1548,51 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B40" s="8">
         <f>B9</f>
         <v>7500</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B41" s="1">
         <f>SUM(B38:B40)</f>
         <v>10759</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B42" s="1"/>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B43" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="B43" s="20" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A44" s="14" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B44" s="16">
         <f>4*E4*B17/60</f>
         <v>2768</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B45" s="8">
         <f>E6*B17/60</f>
         <v>4000</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B46" s="1">
         <f>SUM(B44:B45)</f>
         <v>6768</v>
@@ -1308,8 +1601,8 @@
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:E1"/>
-    <mergeCell ref="G1:L1"/>
     <mergeCell ref="M1:U1"/>
+    <mergeCell ref="G1:K1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>